<commit_message>
proiectul de baza pentru lucrul cu Entity Framework
</commit_message>
<xml_diff>
--- a/SGBD/Prezenta.xlsx
+++ b/SGBD/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\SGBD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A80881-0D61-43BD-A508-F305B9207039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A57BB2-0756-48E0-9745-B8B3E27758B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Nota</t>
   </si>
@@ -148,13 +148,31 @@
   </si>
   <si>
     <t>Roland Roman</t>
+  </si>
+  <si>
+    <t>Catalin Lazar</t>
+  </si>
+  <si>
+    <t>Vlad Brata</t>
+  </si>
+  <si>
+    <t>Ravan Ardeli</t>
+  </si>
+  <si>
+    <t>Vlad Chis</t>
+  </si>
+  <si>
+    <t>Sebastian Pop</t>
+  </si>
+  <si>
+    <t>Cosmin Chira</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,15 +200,8 @@
       <color rgb="FF000000"/>
       <name val="Calibri1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,11 +236,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF9DC3E6"/>
         <bgColor rgb="FF9DC3E6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -411,12 +417,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -477,19 +482,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="8" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Default" xfId="1" xr:uid="{EB53C024-DCAD-4D39-B7BA-74E17CBDBE71}"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -782,7 +782,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -850,43 +850,50 @@
       <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
+      <c r="C3" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="14"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="31"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="29"/>
       <c r="Q3" s="4">
         <f>C3+D3+E3+F3+G3+H3+I3+J3+K3+L3+M3+N3+O3+P3</f>
         <v>1</v>
       </c>
-      <c r="R3" s="32"/>
+      <c r="R3" s="30"/>
     </row>
     <row r="4" spans="2:18">
       <c r="B4" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D4" s="33" t="b">
-        <v>1</v>
-      </c>
+      <c r="C4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="4">
         <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4" s="7"/>
     </row>
@@ -894,17 +901,24 @@
       <c r="B5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="33" t="b">
-        <v>1</v>
-      </c>
+      <c r="C5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
       <c r="J5" s="13"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="4">
         <f>C5+D5+E5+F5+G5+H5+I5+J5+K5+L5+M5+N5+O5+P5</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R5" s="7"/>
     </row>
@@ -912,17 +926,24 @@
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="33" t="b">
-        <v>1</v>
-      </c>
+      <c r="C6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="4">
         <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R6" s="7"/>
     </row>
@@ -930,9 +951,15 @@
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="28" t="b">
-        <v>1</v>
-      </c>
+      <c r="C7" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
       <c r="J7" s="13"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="4">
@@ -943,13 +970,13 @@
     </row>
     <row r="8" spans="2:18">
       <c r="B8" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13"/>
+        <v>41</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
@@ -969,312 +996,430 @@
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="33" t="b">
-        <v>1</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>2</v>
-      </c>
-      <c r="R9" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="R9" s="7"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="33" t="b">
-        <v>1</v>
-      </c>
+      <c r="B10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
       <c r="J10" s="13"/>
-      <c r="P10" s="6"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="16"/>
       <c r="Q10" s="4">
         <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>2</v>
-      </c>
-      <c r="R10" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="R10" s="23"/>
     </row>
     <row r="11" spans="2:18">
       <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="33" t="b">
-        <v>1</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="4">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>2</v>
-      </c>
-      <c r="R11" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="R11" s="8"/>
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="28" t="b">
-        <v>1</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="4">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R12" s="7"/>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="33" t="b">
-        <v>1</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="4">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R13" s="7"/>
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="33" t="b">
-        <v>1</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C14" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
       <c r="J14" s="13"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="4">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14" s="7"/>
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="28" t="b">
-        <v>1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
       <c r="J15" s="13"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="4">
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R15" s="7"/>
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
       <c r="J16" s="13"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
         <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R16" s="7"/>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="34" t="b">
-        <v>1</v>
-      </c>
+      <c r="B17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="16"/>
+      <c r="P17" s="6"/>
       <c r="Q17" s="4">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>2</v>
-      </c>
-      <c r="R17" s="18"/>
+        <v>1</v>
+      </c>
+      <c r="R17" s="7"/>
     </row>
     <row r="18" spans="2:18">
       <c r="B18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="4">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="2:18">
-      <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="33" t="b">
-        <v>1</v>
-      </c>
+      <c r="B19" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
       <c r="J19" s="13"/>
-      <c r="P19" s="6"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="16"/>
       <c r="Q19" s="4">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
-        <v>2</v>
-      </c>
-      <c r="R19" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="R19" s="18"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="34" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="13"/>
+      <c r="B20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D20" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="16"/>
+      <c r="P20" s="6"/>
       <c r="Q20" s="4">
         <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>2</v>
-      </c>
-      <c r="R20" s="23"/>
+        <v>3</v>
+      </c>
+      <c r="R20" s="7"/>
     </row>
     <row r="21" spans="2:18">
       <c r="B21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" s="33" t="b">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F21" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="4">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R21" s="7"/>
     </row>
     <row r="22" spans="2:18">
-      <c r="B22" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" s="33" t="b">
-        <v>1</v>
-      </c>
+      <c r="B22" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
       <c r="J22" s="13"/>
-      <c r="P22" s="6"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="16"/>
       <c r="Q22" s="4">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>2</v>
-      </c>
-      <c r="R22" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="R22" s="23"/>
     </row>
     <row r="23" spans="2:18">
       <c r="B23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="33" t="b">
-        <v>1</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="4">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R23" s="7"/>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="28" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="33" t="b">
-        <v>1</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F24" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
       <c r="J24" s="13"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="4">
         <f>C24+D24+E24+F24+G24+H24+I24+J24+K24+L24+M24+N24+O24+P24</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R24" s="7"/>
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="33" t="b">
-        <v>1</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="4">
@@ -1285,110 +1430,191 @@
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="28" t="b">
-        <v>1</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F26" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
       <c r="J26" s="13"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="4">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>1</v>
-      </c>
-      <c r="R26" s="8"/>
+        <v>4</v>
+      </c>
+      <c r="R26" s="7"/>
     </row>
     <row r="27" spans="2:18">
-      <c r="B27" s="19"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
+      <c r="B27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D27" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E27" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="16"/>
+      <c r="P27" s="6"/>
       <c r="Q27" s="4">
-        <f t="shared" ref="Q24:Q34" si="0">C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>0</v>
-      </c>
-      <c r="R27" s="23"/>
+        <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
+        <v>4</v>
+      </c>
+      <c r="R27" s="7"/>
     </row>
     <row r="28" spans="2:18">
-      <c r="B28" s="3"/>
-      <c r="C28" s="5"/>
+      <c r="B28" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E28" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
       <c r="J28" s="13"/>
       <c r="P28" s="6"/>
       <c r="Q28" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R28" s="8"/>
+        <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
+        <v>2</v>
+      </c>
+      <c r="R28" s="7"/>
     </row>
     <row r="29" spans="2:18">
-      <c r="B29" s="3"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
       <c r="J29" s="13"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R29" s="7"/>
+        <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
+        <v>1</v>
+      </c>
+      <c r="R29" s="8"/>
     </row>
     <row r="30" spans="2:18">
-      <c r="B30" s="3"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
       <c r="J30" s="13"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R30" s="7"/>
+        <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
+        <v>1</v>
+      </c>
+      <c r="R30" s="8"/>
     </row>
     <row r="31" spans="2:18">
-      <c r="B31" s="3"/>
-      <c r="C31" s="5"/>
+      <c r="B31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
       <c r="J31" s="13"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C31+D31+E31+F31+G31+H31+I31+J31+K31+L31+M31+N31+O31+P31</f>
+        <v>1</v>
       </c>
       <c r="R31" s="8"/>
     </row>
     <row r="32" spans="2:18">
-      <c r="B32" s="3"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
       <c r="J32" s="13"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
+        <v>1</v>
       </c>
       <c r="R32" s="7"/>
     </row>
     <row r="33" spans="2:18">
       <c r="B33" s="3"/>
-      <c r="C33" s="5"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
       <c r="J33" s="13"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q29:Q34" si="0">C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
         <v>0</v>
       </c>
       <c r="R33" s="7"/>
     </row>
     <row r="34" spans="2:18">
       <c r="B34" s="3"/>
-      <c r="C34" s="5"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
       <c r="J34" s="13"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="4">
@@ -1399,7 +1625,13 @@
     </row>
     <row r="35" spans="2:18">
       <c r="B35" s="3"/>
-      <c r="C35" s="5"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
       <c r="J35" s="13"/>
       <c r="P35" s="6"/>
       <c r="Q35" s="4">
@@ -1410,7 +1642,13 @@
     </row>
     <row r="36" spans="2:18">
       <c r="B36" s="3"/>
-      <c r="C36" s="5"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
       <c r="J36" s="13"/>
       <c r="P36" s="6"/>
       <c r="Q36" s="4">
@@ -1421,7 +1659,13 @@
     </row>
     <row r="37" spans="2:18">
       <c r="B37" s="3"/>
-      <c r="C37" s="5"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
       <c r="J37" s="13"/>
       <c r="P37" s="6"/>
       <c r="Q37" s="4">
@@ -1432,7 +1676,13 @@
     </row>
     <row r="38" spans="2:18">
       <c r="B38" s="3"/>
-      <c r="C38" s="5"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
       <c r="J38" s="13"/>
       <c r="P38" s="6"/>
       <c r="Q38" s="4">
@@ -1443,7 +1693,13 @@
     </row>
     <row r="39" spans="2:18">
       <c r="B39" s="3"/>
-      <c r="C39" s="5"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
       <c r="J39" s="13"/>
       <c r="P39" s="6"/>
       <c r="Q39" s="4">
@@ -1693,8 +1949,8 @@
       <c r="R59" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R26">
-    <sortCondition ref="B26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R32">
+    <sortCondition ref="B32"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q59">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>

<commit_message>
legatura cu bazza de date finalizata
</commit_message>
<xml_diff>
--- a/SGBD/Prezenta.xlsx
+++ b/SGBD/Prezenta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remus\Documents\GitHub\Facultate_Promotia_2023_2026\SGBD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A57BB2-0756-48E0-9745-B8B3E27758B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4524230-32DA-43AA-9D68-44339CE0AE9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Nota</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Vlad Brata</t>
   </si>
   <si>
-    <t>Ravan Ardeli</t>
-  </si>
-  <si>
     <t>Vlad Chis</t>
   </si>
   <si>
@@ -166,6 +163,12 @@
   </si>
   <si>
     <t>Cosmin Chira</t>
+  </si>
+  <si>
+    <t>Daniel Oistic</t>
+  </si>
+  <si>
+    <t>Razvan Ardeli</t>
   </si>
 </sst>
 </file>
@@ -779,10 +782,10 @@
   <dimension ref="B2:R59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -886,14 +889,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="G4" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="4">
         <f>C4+D4+E4+F4+G4+H4+I4+J4+K4+L4+M4+N4+O4+P4</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R4" s="7"/>
     </row>
@@ -936,14 +941,16 @@
         <v>1</v>
       </c>
       <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="4">
         <f>C6+D6+E6+F6+G6+H6+I6+J6+K6+L6+M6+N6+O6+P6</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R6" s="7"/>
     </row>
@@ -978,7 +985,9 @@
         <v>1</v>
       </c>
       <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="G8" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
@@ -990,13 +999,13 @@
       <c r="P8" s="16"/>
       <c r="Q8" s="4">
         <f>C8+D8+E8+F8+G8+H8+I8+J8+K8+L8+M8+N8+O8+P8</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R8" s="23"/>
     </row>
     <row r="9" spans="2:18">
       <c r="B9" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -1004,54 +1013,45 @@
       <c r="F9" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="4">
         <f>C9+D9+E9+F9+G9+H9+I9+J9+K9+L9+M9+N9+O9+P9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R9" s="7"/>
     </row>
     <row r="10" spans="2:18">
-      <c r="B10" s="19" t="s">
-        <v>38</v>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="C10" s="13"/>
-      <c r="D10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F10" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="16"/>
+      <c r="P10" s="6"/>
       <c r="Q10" s="4">
         <f>C10+D10+E10+F10+G10+H10+I10+J10+K10+L10+M10+N10+O10+P10</f>
-        <v>3</v>
-      </c>
-      <c r="R10" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="R10" s="7"/>
     </row>
     <row r="11" spans="2:18">
-      <c r="B11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="B11" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="13"/>
       <c r="D11" s="13" t="b">
         <v>1</v>
       </c>
@@ -1065,16 +1065,21 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
-      <c r="P11" s="6"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="16"/>
       <c r="Q11" s="4">
         <f>C11+D11+E11+F11+G11+H11+I11+J11+K11+L11+M11+N11+O11+P11</f>
-        <v>4</v>
-      </c>
-      <c r="R11" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="R11" s="23"/>
     </row>
     <row r="12" spans="2:18">
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C12" s="13" t="b">
         <v>1</v>
@@ -1088,20 +1093,22 @@
       <c r="F12" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="4">
         <f>C12+D12+E12+F12+G12+H12+I12+J12+K12+L12+M12+N12+O12+P12</f>
-        <v>4</v>
-      </c>
-      <c r="R12" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="R12" s="8"/>
     </row>
     <row r="13" spans="2:18">
       <c r="B13" s="3" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C13" s="13" t="b">
         <v>1</v>
@@ -1109,31 +1116,39 @@
       <c r="D13" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E13" s="13"/>
+      <c r="E13" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F13" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G13" s="13"/>
+      <c r="G13" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="4">
         <f>C13+D13+E13+F13+G13+H13+I13+J13+K13+L13+M13+N13+O13+P13</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="R13" s="7"/>
     </row>
     <row r="14" spans="2:18">
       <c r="B14" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C14" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="D14" s="13"/>
+      <c r="D14" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
+      <c r="F14" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -1141,22 +1156,20 @@
       <c r="P14" s="6"/>
       <c r="Q14" s="4">
         <f>C14+D14+E14+F14+G14+H14+I14+J14+K14+L14+M14+N14+O14+P14</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R14" s="7"/>
     </row>
     <row r="15" spans="2:18">
       <c r="B15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13" t="b">
-        <v>1</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C15" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
@@ -1164,23 +1177,19 @@
       <c r="P15" s="6"/>
       <c r="Q15" s="4">
         <f>C15+D15+E15+F15+G15+H15+I15+J15+K15+L15+M15+N15+O15+P15</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R15" s="7"/>
     </row>
     <row r="16" spans="2:18">
       <c r="B16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="13" t="b">
-        <v>1</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C16" s="13"/>
       <c r="D16" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E16" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="E16" s="13"/>
       <c r="F16" s="13" t="b">
         <v>1</v>
       </c>
@@ -1191,20 +1200,26 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="4">
         <f>C16+D16+E16+F16+G16+H16+I16+J16+K16+L16+M16+N16+O16+P16</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R16" s="7"/>
     </row>
     <row r="17" spans="2:18">
       <c r="B17" s="3" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="C17" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
+      <c r="D17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
@@ -1212,24 +1227,20 @@
       <c r="P17" s="6"/>
       <c r="Q17" s="4">
         <f>C17+D17+E17+F17+G17+H17+I17+J17+K17+L17+M17+N17+O17+P17</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R17" s="7"/>
     </row>
     <row r="18" spans="2:18">
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C18" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="D18" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="D18" s="13"/>
       <c r="E18" s="13"/>
-      <c r="F18" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="F18" s="13"/>
       <c r="G18" s="13"/>
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
@@ -1237,13 +1248,13 @@
       <c r="P18" s="6"/>
       <c r="Q18" s="4">
         <f>C18+D18+E18+F18+G18+H18+I18+J18+K18+L18+M18+N18+O18+P18</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R18" s="7"/>
     </row>
     <row r="19" spans="2:18">
-      <c r="B19" s="19" t="s">
-        <v>27</v>
+      <c r="B19" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C19" s="13" t="b">
         <v>1</v>
@@ -1251,31 +1262,26 @@
       <c r="D19" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E19" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="E19" s="13"/>
       <c r="F19" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G19" s="13"/>
+      <c r="G19" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="16"/>
+      <c r="P19" s="6"/>
       <c r="Q19" s="4">
         <f>C19+D19+E19+F19+G19+H19+I19+J19+K19+L19+M19+N19+O19+P19</f>
         <v>4</v>
       </c>
-      <c r="R19" s="18"/>
+      <c r="R19" s="7"/>
     </row>
     <row r="20" spans="2:18">
-      <c r="B20" s="3" t="s">
-        <v>30</v>
+      <c r="B20" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="C20" s="13" t="b">
         <v>1</v>
@@ -1286,21 +1292,28 @@
       <c r="E20" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="F20" s="13"/>
+      <c r="F20" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
-      <c r="P20" s="6"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="16"/>
       <c r="Q20" s="4">
         <f>C20+D20+E20+F20+G20+H20+I20+J20+K20+L20+M20+N20+O20+P20</f>
-        <v>3</v>
-      </c>
-      <c r="R20" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="R20" s="18"/>
     </row>
     <row r="21" spans="2:18">
       <c r="B21" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C21" s="13" t="b">
         <v>1</v>
@@ -1311,9 +1324,7 @@
       <c r="E21" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="F21" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="F21" s="13"/>
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
@@ -1321,13 +1332,13 @@
       <c r="P21" s="6"/>
       <c r="Q21" s="4">
         <f>C21+D21+E21+F21+G21+H21+I21+J21+K21+L21+M21+N21+O21+P21</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R21" s="7"/>
     </row>
     <row r="22" spans="2:18">
-      <c r="B22" s="19" t="s">
-        <v>34</v>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C22" s="13" t="b">
         <v>1</v>
@@ -1335,29 +1346,28 @@
       <c r="D22" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E22" s="13"/>
+      <c r="E22" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F22" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="16"/>
+      <c r="P22" s="6"/>
       <c r="Q22" s="4">
         <f>C22+D22+E22+F22+G22+H22+I22+J22+K22+L22+M22+N22+O22+P22</f>
-        <v>3</v>
-      </c>
-      <c r="R22" s="23"/>
+        <v>5</v>
+      </c>
+      <c r="R22" s="7"/>
     </row>
     <row r="23" spans="2:18">
-      <c r="B23" s="3" t="s">
-        <v>21</v>
+      <c r="B23" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="C23" s="13" t="b">
         <v>1</v>
@@ -1365,24 +1375,31 @@
       <c r="D23" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E23" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
-      <c r="P23" s="6"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="16"/>
       <c r="Q23" s="4">
         <f>C23+D23+E23+F23+G23+H23+I23+J23+K23+L23+M23+N23+O23+P23</f>
-        <v>3</v>
-      </c>
-      <c r="R23" s="7"/>
+        <v>4</v>
+      </c>
+      <c r="R23" s="23"/>
     </row>
     <row r="24" spans="2:18">
       <c r="B24" s="3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C24" s="13" t="b">
         <v>1</v>
@@ -1393,10 +1410,10 @@
       <c r="E24" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="F24" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
@@ -1409,55 +1426,59 @@
     </row>
     <row r="25" spans="2:18">
       <c r="B25" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
+        <v>32</v>
+      </c>
+      <c r="C25" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="F25" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G25" s="13"/>
+      <c r="G25" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="4">
         <f>C25+D25+E25+F25+G25+H25+I25+J25+K25+L25+M25+N25+O25+P25</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="R25" s="7"/>
     </row>
     <row r="26" spans="2:18">
       <c r="B26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="D26" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="13" t="b">
-        <v>1</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G26" s="13"/>
+      <c r="G26" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="4">
         <f>C26+D26+E26+F26+G26+H26+I26+J26+K26+L26+M26+N26+O26+P26</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R26" s="7"/>
     </row>
     <row r="27" spans="2:18">
       <c r="B27" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C27" s="13" t="b">
         <v>1</v>
@@ -1471,29 +1492,35 @@
       <c r="F27" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="G27" s="13"/>
+      <c r="G27" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
       <c r="P27" s="6"/>
       <c r="Q27" s="4">
         <f>C27+D27+E27+F27+G27+H27+I27+J27+K27+L27+M27+N27+O27+P27</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R27" s="7"/>
     </row>
     <row r="28" spans="2:18">
       <c r="B28" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C28" s="13"/>
+        <v>23</v>
+      </c>
+      <c r="C28" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="D28" s="13" t="b">
         <v>1</v>
       </c>
       <c r="E28" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="F28" s="13"/>
+      <c r="F28" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
@@ -1501,61 +1528,67 @@
       <c r="P28" s="6"/>
       <c r="Q28" s="4">
         <f>C28+D28+E28+F28+G28+H28+I28+J28+K28+L28+M28+N28+O28+P28</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R28" s="7"/>
     </row>
     <row r="29" spans="2:18">
       <c r="B29" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13" t="b">
-        <v>1</v>
-      </c>
-      <c r="G29" s="13"/>
+      <c r="D29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
       <c r="P29" s="6"/>
       <c r="Q29" s="4">
         <f>C29+D29+E29+F29+G29+H29+I29+J29+K29+L29+M29+N29+O29+P29</f>
-        <v>1</v>
-      </c>
-      <c r="R29" s="8"/>
+        <v>3</v>
+      </c>
+      <c r="R29" s="7"/>
     </row>
     <row r="30" spans="2:18">
       <c r="B30" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="13" t="b">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C30" s="13"/>
       <c r="D30" s="13"/>
       <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="F30" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="4">
         <f>C30+D30+E30+F30+G30+H30+I30+J30+K30+L30+M30+N30+O30+P30</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R30" s="8"/>
     </row>
     <row r="31" spans="2:18">
       <c r="B31" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="13"/>
+        <v>18</v>
+      </c>
+      <c r="C31" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="D31" s="13"/>
-      <c r="E31" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
@@ -1570,14 +1603,14 @@
     </row>
     <row r="32" spans="2:18">
       <c r="B32" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13" t="b">
-        <v>1</v>
-      </c>
+      <c r="E32" s="13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
@@ -1587,22 +1620,26 @@
         <f>C32+D32+E32+F32+G32+H32+I32+J32+K32+L32+M32+N32+O32+P32</f>
         <v>1</v>
       </c>
-      <c r="R32" s="7"/>
+      <c r="R32" s="8"/>
     </row>
     <row r="33" spans="2:18">
-      <c r="B33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="C33" s="13"/>
       <c r="D33" s="13"/>
       <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="F33" s="13" t="b">
+        <v>1</v>
+      </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
       <c r="P33" s="6"/>
       <c r="Q33" s="4">
-        <f t="shared" ref="Q29:Q34" si="0">C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
-        <v>0</v>
+        <f>C33+D33+E33+F33+G33+H33+I33+J33+K33+L33+M33+N33+O33+P33</f>
+        <v>1</v>
       </c>
       <c r="R33" s="7"/>
     </row>
@@ -1618,7 +1655,7 @@
       <c r="J34" s="13"/>
       <c r="P34" s="6"/>
       <c r="Q34" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="Q33:Q34" si="0">C34+D34+E34+F34+G34+H34+I34+J34+K34+L34+M34+N34+O34+P34</f>
         <v>0</v>
       </c>
       <c r="R34" s="7"/>
@@ -1949,8 +1986,8 @@
       <c r="R59" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R32">
-    <sortCondition ref="B32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:R33">
+    <sortCondition ref="B33"/>
   </sortState>
   <conditionalFormatting sqref="Q3:Q59">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">

</xml_diff>